<commit_message>
Added run.bat that runs the api_pixels.py and the pixels_.....xlsm, the macro enabled version of the other excel and can call the run.bat file
</commit_message>
<xml_diff>
--- a/pixels_all_buy_and_craft.xlsx
+++ b/pixels_all_buy_and_craft.xlsx
@@ -2,15 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
-  <workbookPr/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\others\pixels_new\PixelsSheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A04ABBB-C1CC-453A-B62E-8FE2CA4E8A46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A15E859-FF67-4A07-8AA2-25CBAA1EC9A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="10" r:id="rId1"/>
@@ -5502,6 +5502,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1F93B273-2E2B-484F-94FD-BA69EBCD3234}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -6326,6 +6327,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D65AEE96-FD81-433F-873C-D44F834FAE43}">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:O90"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11302,6 +11304,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6CEF616-CFB1-43BC-A42C-BACF725A22DA}">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11337,6 +11340,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC2F28ED-26A7-48D9-AF17-5E033E78693B}">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -11503,6 +11507,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{362E9DC3-AF61-4F39-A8A0-486E7B0BBE9C}">
+  <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:B69"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -12077,6 +12082,7 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{922E046B-8AF6-41E6-B423-008BA81D6DD3}">
+  <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:C105"/>
   <sheetViews>
     <sheetView topLeftCell="A57" workbookViewId="0">
@@ -13358,9 +13364,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E515E31-052A-428F-AC42-5FA84063035A}">
+  <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:L61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="S45" sqref="S45"/>
     </sheetView>
   </sheetViews>
@@ -16166,6 +16173,7 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B97CE9CB-432F-4DEE-AA5D-0F831EE3ABB5}">
+  <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:D49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -16980,9 +16988,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D8F98C8-A1C7-48C1-9D4F-332B9CE06CB7}">
+  <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>